<commit_message>
Added updated macro-financial datasets for France and US
</commit_message>
<xml_diff>
--- a/CPI_France_FRED.xlsx
+++ b/CPI_France_FRED.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yesminehachana/Desktop/Classes/Dauphine/2nd Semester/Macroeconomics MATLAB Project/Repository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53DD72E-BA8F-C64E-81F7-C69E1EF324D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B3C58A-4966-7745-A4C6-568AE0D929E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>FRED Graph Observations</t>
   </si>
@@ -50,16 +50,18 @@
     <t>Data Updated: 2024-04-10</t>
   </si>
   <si>
-    <t>observation_date</t>
+    <t>Consumer Price Index France</t>
+  </si>
+  <si>
+    <t>Quarter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000000000000"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -122,7 +124,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +432,7 @@
   <dimension ref="A1:B276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -441,10 +443,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>